<commit_message>
changed calculation of optimal path length to at the origin. refactored network. add 3 options for dealing with unsolvability
</commit_message>
<xml_diff>
--- a/Logs/test_new/testing_episode_output.xlsx
+++ b/Logs/test_new/testing_episode_output.xlsx
@@ -383,7 +383,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D95"/>
+  <dimension ref="A1:D97"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -405,262 +405,262 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2">
-        <v>-1.279999971389771</v>
+        <v>-1.189000010490417</v>
       </c>
       <c r="B2">
-        <v>0.25</v>
+        <v>1</v>
       </c>
       <c r="C2">
-        <v>1.029999971389771</v>
+        <v>0.1890000104904175</v>
       </c>
       <c r="D2">
-        <v>5.119999885559082</v>
+        <v>1.189000010490417</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3">
-        <v>-1.450000047683716</v>
+        <v>-3.424000024795532</v>
       </c>
       <c r="B3">
-        <v>0.25</v>
+        <v>1</v>
       </c>
       <c r="C3">
-        <v>1.200000047683716</v>
+        <v>2.424000024795532</v>
       </c>
       <c r="D3">
-        <v>5.800000190734863</v>
+        <v>3.424000024795532</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4">
-        <v>-1.049999952316284</v>
+        <v>-5.335999965667725</v>
       </c>
       <c r="B4">
-        <v>0.2599999904632568</v>
+        <v>1.289999961853027</v>
       </c>
       <c r="C4">
-        <v>0.7899999618530273</v>
+        <v>4.046000003814697</v>
       </c>
       <c r="D4">
-        <v>4.038461685180664</v>
+        <v>4.136434078216553</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5">
-        <v>-1</v>
+        <v>-2.858999967575073</v>
       </c>
       <c r="B5">
-        <v>0.3100000023841858</v>
+        <v>1.054999947547913</v>
       </c>
       <c r="C5">
-        <v>0.6899999976158142</v>
+        <v>1.804000020027161</v>
       </c>
       <c r="D5">
-        <v>3.225806474685669</v>
+        <v>2.709952592849731</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6">
-        <v>-0.6499999761581421</v>
+        <v>-1.470999956130981</v>
       </c>
       <c r="B6">
-        <v>0.2599999904632568</v>
+        <v>1.342000007629395</v>
       </c>
       <c r="C6">
-        <v>0.3899999856948853</v>
+        <v>0.1289999485015869</v>
       </c>
       <c r="D6">
-        <v>2.5</v>
+        <v>1.09612512588501</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7">
-        <v>-0.3700000047683716</v>
+        <v>-1.570000052452087</v>
       </c>
       <c r="B7">
-        <v>0.3400000035762787</v>
+        <v>1.080000042915344</v>
       </c>
       <c r="C7">
-        <v>0.0300000011920929</v>
+        <v>0.4900000095367432</v>
       </c>
       <c r="D7">
-        <v>1.088235259056091</v>
+        <v>1.453703641891479</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8">
-        <v>-0.3899999856948853</v>
+        <v>-1.024999976158142</v>
       </c>
       <c r="B8">
-        <v>0.2700000107288361</v>
+        <v>1.024999976158142</v>
       </c>
       <c r="C8">
-        <v>0.1199999749660492</v>
+        <v>0</v>
       </c>
       <c r="D8">
-        <v>1.444444298744202</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9">
-        <v>-0.2599999904632568</v>
+        <v>-11.27299976348877</v>
       </c>
       <c r="B9">
-        <v>0.2599999904632568</v>
+        <v>1.526999950408936</v>
       </c>
       <c r="C9">
-        <v>0</v>
+        <v>9.746000289916992</v>
       </c>
       <c r="D9">
-        <v>1</v>
+        <v>7.382449150085449</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10">
-        <v>-1.860000014305115</v>
+        <v>-1.353999972343445</v>
       </c>
       <c r="B10">
-        <v>0.3799999952316284</v>
+        <v>1.291000008583069</v>
       </c>
       <c r="C10">
-        <v>1.480000019073486</v>
+        <v>0.06299996376037598</v>
       </c>
       <c r="D10">
-        <v>4.894736766815186</v>
+        <v>1.048799395561218</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11">
-        <v>-0.6800000071525574</v>
+        <v>-2.108999967575073</v>
       </c>
       <c r="B11">
-        <v>0.3600000143051147</v>
+        <v>1</v>
       </c>
       <c r="C11">
-        <v>0.3199999928474426</v>
+        <v>1.108999967575073</v>
       </c>
       <c r="D11">
-        <v>1.888888835906982</v>
+        <v>2.108999967575073</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12">
-        <v>-1</v>
+        <v>-5.581999778747559</v>
       </c>
       <c r="B12">
-        <v>0.2899999916553497</v>
+        <v>1.342000007629395</v>
       </c>
       <c r="C12">
-        <v>0.7100000381469727</v>
+        <v>4.239999771118164</v>
       </c>
       <c r="D12">
-        <v>3.448276042938232</v>
+        <v>4.159463405609131</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13">
-        <v>-1</v>
+        <v>-2.453000068664551</v>
       </c>
       <c r="B13">
-        <v>0.3300000131130219</v>
+        <v>1.154999971389771</v>
       </c>
       <c r="C13">
-        <v>0.6699999570846558</v>
+        <v>1.29800009727478</v>
       </c>
       <c r="D13">
-        <v>3.030303001403809</v>
+        <v>2.123809576034546</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="A14">
-        <v>-1</v>
+        <v>-2.470999956130981</v>
       </c>
       <c r="B14">
-        <v>0.3400000035762787</v>
+        <v>1.235999941825867</v>
       </c>
       <c r="C14">
-        <v>0.6599999666213989</v>
+        <v>1.235000014305115</v>
       </c>
       <c r="D14">
-        <v>2.941176414489746</v>
+        <v>1.999191045761108</v>
       </c>
     </row>
     <row r="15" spans="1:4">
       <c r="A15">
-        <v>-1</v>
+        <v>-1.51800000667572</v>
       </c>
       <c r="B15">
-        <v>0.3400000035762787</v>
+        <v>1.51800000667572</v>
       </c>
       <c r="C15">
-        <v>0.6599999666213989</v>
+        <v>0</v>
       </c>
       <c r="D15">
-        <v>2.941176414489746</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:4">
       <c r="A16">
-        <v>-1</v>
+        <v>-6.061999797821045</v>
       </c>
       <c r="B16">
-        <v>0.300000011920929</v>
+        <v>1.195999979972839</v>
       </c>
       <c r="C16">
-        <v>0.699999988079071</v>
+        <v>4.865999698638916</v>
       </c>
       <c r="D16">
-        <v>3.333333253860474</v>
+        <v>5.068561553955078</v>
       </c>
     </row>
     <row r="17" spans="1:4">
       <c r="A17">
-        <v>-1.320000052452087</v>
+        <v>-2.710999965667725</v>
       </c>
       <c r="B17">
-        <v>0.3700000047683716</v>
+        <v>1.447000026702881</v>
       </c>
       <c r="C17">
-        <v>0.9500000476837158</v>
+        <v>1.263999938964844</v>
       </c>
       <c r="D17">
-        <v>3.567567586898804</v>
+        <v>1.873531341552734</v>
       </c>
     </row>
     <row r="18" spans="1:4">
       <c r="A18">
-        <v>-2.160000085830688</v>
+        <v>-1</v>
       </c>
       <c r="B18">
-        <v>0.2899999916553497</v>
+        <v>1</v>
       </c>
       <c r="C18">
-        <v>1.870000123977661</v>
+        <v>0</v>
       </c>
       <c r="D18">
-        <v>7.448276519775391</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:4">
       <c r="A19">
-        <v>-1.429999947547913</v>
+        <v>-1.753999948501587</v>
       </c>
       <c r="B19">
-        <v>0.300000011920929</v>
+        <v>1</v>
       </c>
       <c r="C19">
-        <v>1.129999876022339</v>
+        <v>0.7539999485015869</v>
       </c>
       <c r="D19">
-        <v>4.766666412353516</v>
+        <v>1.753999948501587</v>
       </c>
     </row>
     <row r="20" spans="1:4">
       <c r="A20">
-        <v>-0.3600000143051147</v>
+        <v>-1.241999983787537</v>
       </c>
       <c r="B20">
-        <v>0.3600000143051147</v>
+        <v>1.241999983787537</v>
       </c>
       <c r="C20">
         <v>0</v>
@@ -671,30 +671,30 @@
     </row>
     <row r="21" spans="1:4">
       <c r="A21">
-        <v>-1.950000047683716</v>
+        <v>-1.975000023841858</v>
       </c>
       <c r="B21">
-        <v>0.3600000143051147</v>
+        <v>1.631999969482422</v>
       </c>
       <c r="C21">
-        <v>1.590000033378601</v>
+        <v>0.343000054359436</v>
       </c>
       <c r="D21">
-        <v>5.416666507720947</v>
+        <v>1.210171580314636</v>
       </c>
     </row>
     <row r="22" spans="1:4">
       <c r="A22">
-        <v>-0.6800000071525574</v>
+        <v>-1.832000017166138</v>
       </c>
       <c r="B22">
-        <v>0.3600000143051147</v>
+        <v>1.832000017166138</v>
       </c>
       <c r="C22">
-        <v>0.3199999928474426</v>
+        <v>0</v>
       </c>
       <c r="D22">
-        <v>1.888888835906982</v>
+        <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:4">
@@ -702,63 +702,63 @@
         <v>-1</v>
       </c>
       <c r="B23">
-        <v>0.300000011920929</v>
+        <v>1</v>
       </c>
       <c r="C23">
-        <v>0.699999988079071</v>
+        <v>0</v>
       </c>
       <c r="D23">
-        <v>3.333333253860474</v>
+        <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:4">
       <c r="A24">
-        <v>-0.4399999976158142</v>
+        <v>-2.786999940872192</v>
       </c>
       <c r="B24">
-        <v>0.2700000107288361</v>
+        <v>1.023000001907349</v>
       </c>
       <c r="C24">
-        <v>0.1699999868869781</v>
+        <v>1.763999938964844</v>
       </c>
       <c r="D24">
-        <v>1.629629611968994</v>
+        <v>2.724340200424194</v>
       </c>
     </row>
     <row r="25" spans="1:4">
       <c r="A25">
-        <v>-0.5099999904632568</v>
+        <v>-1.414000034332275</v>
       </c>
       <c r="B25">
-        <v>0.2700000107288361</v>
+        <v>1.414000034332275</v>
       </c>
       <c r="C25">
-        <v>0.2399999797344208</v>
+        <v>0</v>
       </c>
       <c r="D25">
-        <v>1.888888835906982</v>
+        <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:4">
       <c r="A26">
-        <v>-1</v>
+        <v>-4.706999778747559</v>
       </c>
       <c r="B26">
-        <v>0.3100000023841858</v>
+        <v>1.391999959945679</v>
       </c>
       <c r="C26">
-        <v>0.6899999976158142</v>
+        <v>3.31499981880188</v>
       </c>
       <c r="D26">
-        <v>3.225806474685669</v>
+        <v>3.381465435028076</v>
       </c>
     </row>
     <row r="27" spans="1:4">
       <c r="A27">
-        <v>-0.4600000083446503</v>
+        <v>-1</v>
       </c>
       <c r="B27">
-        <v>0.4600000083446503</v>
+        <v>1</v>
       </c>
       <c r="C27">
         <v>0</v>
@@ -769,220 +769,220 @@
     </row>
     <row r="28" spans="1:4">
       <c r="A28">
-        <v>-1</v>
+        <v>-2.266000032424927</v>
       </c>
       <c r="B28">
-        <v>0.3100000023841858</v>
+        <v>1.631999969482422</v>
       </c>
       <c r="C28">
-        <v>0.6899999976158142</v>
+        <v>0.6340000629425049</v>
       </c>
       <c r="D28">
-        <v>3.225806474685669</v>
+        <v>1.388480424880981</v>
       </c>
     </row>
     <row r="29" spans="1:4">
       <c r="A29">
-        <v>-1.269999980926514</v>
+        <v>-1</v>
       </c>
       <c r="B29">
-        <v>0.2599999904632568</v>
+        <v>1</v>
       </c>
       <c r="C29">
-        <v>1.009999990463257</v>
+        <v>0</v>
       </c>
       <c r="D29">
-        <v>4.884615421295166</v>
+        <v>1</v>
       </c>
     </row>
     <row r="30" spans="1:4">
       <c r="A30">
-        <v>-0.3899999856948853</v>
+        <v>-1</v>
       </c>
       <c r="B30">
-        <v>0.2599999904632568</v>
+        <v>1</v>
       </c>
       <c r="C30">
-        <v>0.1299999952316284</v>
+        <v>0</v>
       </c>
       <c r="D30">
-        <v>1.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="31" spans="1:4">
       <c r="A31">
-        <v>-1.330000042915344</v>
+        <v>-6.061999797821045</v>
       </c>
       <c r="B31">
-        <v>0.3199999928474426</v>
+        <v>2.411999940872192</v>
       </c>
       <c r="C31">
-        <v>1.009999990463257</v>
+        <v>3.649999856948853</v>
       </c>
       <c r="D31">
-        <v>4.15625</v>
+        <v>2.513267040252686</v>
       </c>
     </row>
     <row r="32" spans="1:4">
       <c r="A32">
-        <v>-2.410000085830688</v>
+        <v>-5.438000202178955</v>
       </c>
       <c r="B32">
-        <v>0.4699999988079071</v>
+        <v>1</v>
       </c>
       <c r="C32">
-        <v>1.940000057220459</v>
+        <v>4.438000202178955</v>
       </c>
       <c r="D32">
-        <v>5.127659797668457</v>
+        <v>5.438000202178955</v>
       </c>
     </row>
     <row r="33" spans="1:4">
       <c r="A33">
-        <v>-1.450000047683716</v>
+        <v>-6.656000137329102</v>
       </c>
       <c r="B33">
-        <v>0.3600000143051147</v>
+        <v>1.664000034332275</v>
       </c>
       <c r="C33">
-        <v>1.090000033378601</v>
+        <v>4.992000102996826</v>
       </c>
       <c r="D33">
-        <v>4.027777671813965</v>
+        <v>4</v>
       </c>
     </row>
     <row r="34" spans="1:4">
       <c r="A34">
-        <v>-5.570000171661377</v>
+        <v>-3.414000034332275</v>
       </c>
       <c r="B34">
-        <v>0.3700000047683716</v>
+        <v>1.414000034332275</v>
       </c>
       <c r="C34">
-        <v>5.200000286102295</v>
+        <v>2</v>
       </c>
       <c r="D34">
-        <v>15.05405426025391</v>
+        <v>2.414427042007446</v>
       </c>
     </row>
     <row r="35" spans="1:4">
       <c r="A35">
-        <v>-1.549999952316284</v>
+        <v>-2.290999889373779</v>
       </c>
       <c r="B35">
-        <v>0.4199999868869781</v>
+        <v>1.154000043869019</v>
       </c>
       <c r="C35">
-        <v>1.129999995231628</v>
+        <v>1.136999845504761</v>
       </c>
       <c r="D35">
-        <v>3.690476179122925</v>
+        <v>1.985268473625183</v>
       </c>
     </row>
     <row r="36" spans="1:4">
       <c r="A36">
-        <v>-2.210000038146973</v>
+        <v>-1.174999952316284</v>
       </c>
       <c r="B36">
-        <v>0.6000000238418579</v>
+        <v>1.174999952316284</v>
       </c>
       <c r="C36">
-        <v>1.610000014305115</v>
+        <v>0</v>
       </c>
       <c r="D36">
-        <v>3.683333158493042</v>
+        <v>1</v>
       </c>
     </row>
     <row r="37" spans="1:4">
       <c r="A37">
-        <v>-1.25</v>
+        <v>-1.730000019073486</v>
       </c>
       <c r="B37">
-        <v>0.3499999940395355</v>
+        <v>1.730000019073486</v>
       </c>
       <c r="C37">
-        <v>0.8999999761581421</v>
+        <v>0</v>
       </c>
       <c r="D37">
-        <v>3.571428537368774</v>
+        <v>1</v>
       </c>
     </row>
     <row r="38" spans="1:4">
       <c r="A38">
-        <v>-0.4000000059604645</v>
+        <v>-1</v>
       </c>
       <c r="B38">
-        <v>0.3600000143051147</v>
+        <v>1</v>
       </c>
       <c r="C38">
-        <v>0.03999999165534973</v>
+        <v>0</v>
       </c>
       <c r="D38">
-        <v>1.111111044883728</v>
+        <v>1</v>
       </c>
     </row>
     <row r="39" spans="1:4">
       <c r="A39">
-        <v>-0.4900000095367432</v>
+        <v>-4.215000152587891</v>
       </c>
       <c r="B39">
-        <v>0.2700000107288361</v>
+        <v>1</v>
       </c>
       <c r="C39">
-        <v>0.2199999988079071</v>
+        <v>3.215000152587891</v>
       </c>
       <c r="D39">
-        <v>1.814814805984497</v>
+        <v>4.215000152587891</v>
       </c>
     </row>
     <row r="40" spans="1:4">
       <c r="A40">
-        <v>-4.429999828338623</v>
+        <v>-14.21100044250488</v>
       </c>
       <c r="B40">
-        <v>0.3300000131130219</v>
+        <v>1.5</v>
       </c>
       <c r="C40">
-        <v>4.099999904632568</v>
+        <v>12.71100044250488</v>
       </c>
       <c r="D40">
-        <v>13.424241065979</v>
+        <v>9.473999977111816</v>
       </c>
     </row>
     <row r="41" spans="1:4">
       <c r="A41">
-        <v>-3</v>
+        <v>-1.447000026702881</v>
       </c>
       <c r="B41">
-        <v>0.3400000035762787</v>
+        <v>1.447000026702881</v>
       </c>
       <c r="C41">
-        <v>2.660000085830688</v>
+        <v>0</v>
       </c>
       <c r="D41">
-        <v>8.823529243469238</v>
+        <v>1</v>
       </c>
     </row>
     <row r="42" spans="1:4">
       <c r="A42">
-        <v>-0.6200000047683716</v>
+        <v>-1.580999970436096</v>
       </c>
       <c r="B42">
-        <v>0.25</v>
+        <v>1.580999970436096</v>
       </c>
       <c r="C42">
-        <v>0.3700000047683716</v>
+        <v>0</v>
       </c>
       <c r="D42">
-        <v>2.480000019073486</v>
+        <v>1</v>
       </c>
     </row>
     <row r="43" spans="1:4">
       <c r="A43">
-        <v>-0.4000000059604645</v>
+        <v>-1</v>
       </c>
       <c r="B43">
-        <v>0.4000000059604645</v>
+        <v>1</v>
       </c>
       <c r="C43">
         <v>0</v>
@@ -993,10 +993,10 @@
     </row>
     <row r="44" spans="1:4">
       <c r="A44">
-        <v>-1</v>
+        <v>-1.353999972343445</v>
       </c>
       <c r="B44">
-        <v>1</v>
+        <v>1.353999972343445</v>
       </c>
       <c r="C44">
         <v>0</v>
@@ -1007,72 +1007,72 @@
     </row>
     <row r="45" spans="1:4">
       <c r="A45">
-        <v>-1</v>
+        <v>-11.38300037384033</v>
       </c>
       <c r="B45">
-        <v>0.3199999928474426</v>
+        <v>2.21399998664856</v>
       </c>
       <c r="C45">
-        <v>0.6800000071525574</v>
+        <v>9.169000625610352</v>
       </c>
       <c r="D45">
-        <v>3.125</v>
+        <v>5.141373157501221</v>
       </c>
     </row>
     <row r="46" spans="1:4">
       <c r="A46">
-        <v>-2.779999971389771</v>
+        <v>-5.875</v>
       </c>
       <c r="B46">
-        <v>0.25</v>
+        <v>1.601999998092651</v>
       </c>
       <c r="C46">
-        <v>2.529999971389771</v>
+        <v>4.27299976348877</v>
       </c>
       <c r="D46">
-        <v>11.11999988555908</v>
+        <v>3.667290925979614</v>
       </c>
     </row>
     <row r="47" spans="1:4">
       <c r="A47">
-        <v>-1.379999995231628</v>
+        <v>-3.996000051498413</v>
       </c>
       <c r="B47">
-        <v>0.3100000023841858</v>
+        <v>1.54200005531311</v>
       </c>
       <c r="C47">
-        <v>1.069999933242798</v>
+        <v>2.453999996185303</v>
       </c>
       <c r="D47">
-        <v>4.451612949371338</v>
+        <v>2.591439723968506</v>
       </c>
     </row>
     <row r="48" spans="1:4">
       <c r="A48">
-        <v>-1</v>
+        <v>-2.996000051498413</v>
       </c>
       <c r="B48">
-        <v>0.2800000011920929</v>
+        <v>1.54200005531311</v>
       </c>
       <c r="C48">
-        <v>0.7200000286102295</v>
+        <v>1.453999996185303</v>
       </c>
       <c r="D48">
-        <v>3.571428537368774</v>
+        <v>1.942931175231934</v>
       </c>
     </row>
     <row r="49" spans="1:4">
       <c r="A49">
-        <v>-1</v>
+        <v>-1.151000022888184</v>
       </c>
       <c r="B49">
-        <v>0.4399999976158142</v>
+        <v>1.151000022888184</v>
       </c>
       <c r="C49">
-        <v>0.5600000023841858</v>
+        <v>0</v>
       </c>
       <c r="D49">
-        <v>2.272727251052856</v>
+        <v>1</v>
       </c>
     </row>
     <row r="50" spans="1:4">
@@ -1080,189 +1080,189 @@
         <v>-1</v>
       </c>
       <c r="B50">
-        <v>0.3100000023841858</v>
+        <v>1</v>
       </c>
       <c r="C50">
-        <v>0.6899999976158142</v>
+        <v>0</v>
       </c>
       <c r="D50">
-        <v>3.225806474685669</v>
+        <v>1</v>
       </c>
     </row>
     <row r="51" spans="1:4">
       <c r="A51">
-        <v>-1</v>
+        <v>-4.789000034332275</v>
       </c>
       <c r="B51">
-        <v>0.3499999940395355</v>
+        <v>1.894999980926514</v>
       </c>
       <c r="C51">
-        <v>0.6499999761581421</v>
+        <v>2.894000053405762</v>
       </c>
       <c r="D51">
-        <v>2.857142925262451</v>
+        <v>2.527176856994629</v>
       </c>
     </row>
     <row r="52" spans="1:4">
       <c r="A52">
-        <v>-1.580000042915344</v>
+        <v>-2.115000009536743</v>
       </c>
       <c r="B52">
-        <v>0.3100000023841858</v>
+        <v>1.200000047683716</v>
       </c>
       <c r="C52">
-        <v>1.269999980926514</v>
+        <v>0.9149999618530273</v>
       </c>
       <c r="D52">
-        <v>5.096774101257324</v>
+        <v>1.762499928474426</v>
       </c>
     </row>
     <row r="53" spans="1:4">
       <c r="A53">
-        <v>-1.470000028610229</v>
+        <v>-1.526999950408936</v>
       </c>
       <c r="B53">
-        <v>0.2800000011920929</v>
+        <v>1.322000026702881</v>
       </c>
       <c r="C53">
-        <v>1.190000057220459</v>
+        <v>0.2049999237060547</v>
       </c>
       <c r="D53">
-        <v>5.25</v>
+        <v>1.155068039894104</v>
       </c>
     </row>
     <row r="54" spans="1:4">
       <c r="A54">
-        <v>-1</v>
+        <v>-5.551000118255615</v>
       </c>
       <c r="B54">
-        <v>0.3899999856948853</v>
+        <v>1.33299994468689</v>
       </c>
       <c r="C54">
-        <v>0.6100000143051147</v>
+        <v>4.218000411987305</v>
       </c>
       <c r="D54">
-        <v>2.564102649688721</v>
+        <v>4.164291381835938</v>
       </c>
     </row>
     <row r="55" spans="1:4">
       <c r="A55">
-        <v>-2.410000085830688</v>
+        <v>-3.398000001907349</v>
       </c>
       <c r="B55">
-        <v>0.2899999916553497</v>
+        <v>1.116000056266785</v>
       </c>
       <c r="C55">
-        <v>2.120000123977661</v>
+        <v>2.282000064849854</v>
       </c>
       <c r="D55">
-        <v>8.310345649719238</v>
+        <v>3.044802665710449</v>
       </c>
     </row>
     <row r="56" spans="1:4">
       <c r="A56">
-        <v>-0.8100000023841858</v>
+        <v>-1</v>
       </c>
       <c r="B56">
-        <v>0.3100000023841858</v>
+        <v>1</v>
       </c>
       <c r="C56">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="D56">
-        <v>2.612903118133545</v>
+        <v>1</v>
       </c>
     </row>
     <row r="57" spans="1:4">
       <c r="A57">
-        <v>-0.4399999976158142</v>
+        <v>-3.845999956130981</v>
       </c>
       <c r="B57">
-        <v>0.4099999964237213</v>
+        <v>1.315999984741211</v>
       </c>
       <c r="C57">
-        <v>0.0300000011920929</v>
+        <v>2.529999971389771</v>
       </c>
       <c r="D57">
-        <v>1.073170781135559</v>
+        <v>2.922492504119873</v>
       </c>
     </row>
     <row r="58" spans="1:4">
       <c r="A58">
-        <v>-1</v>
+        <v>-2.030999898910522</v>
       </c>
       <c r="B58">
-        <v>0.25</v>
+        <v>1</v>
       </c>
       <c r="C58">
-        <v>0.75</v>
+        <v>1.030999898910522</v>
       </c>
       <c r="D58">
-        <v>4</v>
+        <v>2.030999898910522</v>
       </c>
     </row>
     <row r="59" spans="1:4">
       <c r="A59">
-        <v>-1</v>
+        <v>-4.22700023651123</v>
       </c>
       <c r="B59">
-        <v>0.3300000131130219</v>
+        <v>1.194000005722046</v>
       </c>
       <c r="C59">
-        <v>0.6699999570846558</v>
+        <v>3.033000230789185</v>
       </c>
       <c r="D59">
-        <v>3.030303001403809</v>
+        <v>3.540201187133789</v>
       </c>
     </row>
     <row r="60" spans="1:4">
       <c r="A60">
-        <v>-1</v>
+        <v>-2.61899995803833</v>
       </c>
       <c r="B60">
-        <v>0.2599999904632568</v>
+        <v>1.254999995231628</v>
       </c>
       <c r="C60">
-        <v>0.7400000095367432</v>
+        <v>1.363999962806702</v>
       </c>
       <c r="D60">
-        <v>3.846153974533081</v>
+        <v>2.086852550506592</v>
       </c>
     </row>
     <row r="61" spans="1:4">
       <c r="A61">
-        <v>-1</v>
+        <v>-17.92200088500977</v>
       </c>
       <c r="B61">
-        <v>0.2800000011920929</v>
+        <v>1.526999950408936</v>
       </c>
       <c r="C61">
-        <v>0.7200000286102295</v>
+        <v>16.39500045776367</v>
       </c>
       <c r="D61">
-        <v>3.571428537368774</v>
+        <v>11.73674011230469</v>
       </c>
     </row>
     <row r="62" spans="1:4">
       <c r="A62">
-        <v>-2.240000009536743</v>
+        <v>-2.176000118255615</v>
       </c>
       <c r="B62">
-        <v>1</v>
+        <v>1.452000021934509</v>
       </c>
       <c r="C62">
-        <v>1.240000009536743</v>
+        <v>0.724000096321106</v>
       </c>
       <c r="D62">
-        <v>2.240000009536743</v>
+        <v>1.49862265586853</v>
       </c>
     </row>
     <row r="63" spans="1:4">
       <c r="A63">
-        <v>-0.3700000047683716</v>
+        <v>-1</v>
       </c>
       <c r="B63">
-        <v>0.3700000047683716</v>
+        <v>1</v>
       </c>
       <c r="C63">
         <v>0</v>
@@ -1273,30 +1273,30 @@
     </row>
     <row r="64" spans="1:4">
       <c r="A64">
-        <v>-4.480000019073486</v>
+        <v>-1</v>
       </c>
       <c r="B64">
-        <v>0.3799999952316284</v>
+        <v>1</v>
       </c>
       <c r="C64">
-        <v>4.099999904632568</v>
+        <v>0</v>
       </c>
       <c r="D64">
-        <v>11.78947353363037</v>
+        <v>1</v>
       </c>
     </row>
     <row r="65" spans="1:4">
       <c r="A65">
-        <v>-0.5400000214576721</v>
+        <v>-3.943000078201294</v>
       </c>
       <c r="B65">
-        <v>0.3600000143051147</v>
+        <v>1.631999969482422</v>
       </c>
       <c r="C65">
-        <v>0.1800000071525574</v>
+        <v>2.311000108718872</v>
       </c>
       <c r="D65">
-        <v>1.5</v>
+        <v>2.416054010391235</v>
       </c>
     </row>
     <row r="66" spans="1:4">
@@ -1304,217 +1304,217 @@
         <v>-1</v>
       </c>
       <c r="B66">
-        <v>0.25</v>
+        <v>1</v>
       </c>
       <c r="C66">
-        <v>0.75</v>
+        <v>0</v>
       </c>
       <c r="D66">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="67" spans="1:4">
       <c r="A67">
-        <v>-1.389999985694885</v>
+        <v>-2.431999921798706</v>
       </c>
       <c r="B67">
-        <v>1</v>
+        <v>1.496999979019165</v>
       </c>
       <c r="C67">
-        <v>0.3899999856948853</v>
+        <v>0.934999942779541</v>
       </c>
       <c r="D67">
-        <v>1.389999985694885</v>
+        <v>1.624582409858704</v>
       </c>
     </row>
     <row r="68" spans="1:4">
       <c r="A68">
-        <v>-1.350000023841858</v>
+        <v>-2.86899995803833</v>
       </c>
       <c r="B68">
-        <v>0.3499999940395355</v>
+        <v>1</v>
       </c>
       <c r="C68">
-        <v>1</v>
+        <v>1.86899995803833</v>
       </c>
       <c r="D68">
-        <v>3.857142925262451</v>
+        <v>2.86899995803833</v>
       </c>
     </row>
     <row r="69" spans="1:4">
       <c r="A69">
-        <v>-0.3899999856948853</v>
+        <v>-1.75</v>
       </c>
       <c r="B69">
-        <v>0.3499999940395355</v>
+        <v>1.266000032424927</v>
       </c>
       <c r="C69">
-        <v>0.03999999165534973</v>
+        <v>0.4839999675750732</v>
       </c>
       <c r="D69">
-        <v>1.114285707473755</v>
+        <v>1.382306456565857</v>
       </c>
     </row>
     <row r="70" spans="1:4">
       <c r="A70">
-        <v>-5.480000019073486</v>
+        <v>-1</v>
       </c>
       <c r="B70">
         <v>1</v>
       </c>
       <c r="C70">
-        <v>4.480000019073486</v>
+        <v>0</v>
       </c>
       <c r="D70">
-        <v>5.480000019073486</v>
+        <v>1</v>
       </c>
     </row>
     <row r="71" spans="1:4">
       <c r="A71">
-        <v>-1</v>
+        <v>-5.629000186920166</v>
       </c>
       <c r="B71">
-        <v>0.300000011920929</v>
+        <v>2.493000030517578</v>
       </c>
       <c r="C71">
-        <v>0.699999988079071</v>
+        <v>3.136000156402588</v>
       </c>
       <c r="D71">
-        <v>3.333333253860474</v>
+        <v>2.257922172546387</v>
       </c>
     </row>
     <row r="72" spans="1:4">
       <c r="A72">
-        <v>-0.3400000035762787</v>
+        <v>-2.730000019073486</v>
       </c>
       <c r="B72">
-        <v>0.3400000035762787</v>
+        <v>1</v>
       </c>
       <c r="C72">
-        <v>0</v>
+        <v>1.730000019073486</v>
       </c>
       <c r="D72">
-        <v>1</v>
+        <v>2.730000019073486</v>
       </c>
     </row>
     <row r="73" spans="1:4">
       <c r="A73">
-        <v>-0.3600000143051147</v>
+        <v>-3.111000061035156</v>
       </c>
       <c r="B73">
-        <v>0.3600000143051147</v>
+        <v>1.172000050544739</v>
       </c>
       <c r="C73">
-        <v>0</v>
+        <v>1.939000010490417</v>
       </c>
       <c r="D73">
-        <v>1</v>
+        <v>2.654436826705933</v>
       </c>
     </row>
     <row r="74" spans="1:4">
       <c r="A74">
-        <v>-1</v>
+        <v>-1.447000026702881</v>
       </c>
       <c r="B74">
-        <v>0.2599999904632568</v>
+        <v>1.447000026702881</v>
       </c>
       <c r="C74">
-        <v>0.7400000095367432</v>
+        <v>0</v>
       </c>
       <c r="D74">
-        <v>3.846153974533081</v>
+        <v>1</v>
       </c>
     </row>
     <row r="75" spans="1:4">
       <c r="A75">
-        <v>-0.7900000214576721</v>
+        <v>-1</v>
       </c>
       <c r="B75">
-        <v>0.3100000023841858</v>
+        <v>1</v>
       </c>
       <c r="C75">
-        <v>0.4800000190734863</v>
+        <v>0</v>
       </c>
       <c r="D75">
-        <v>2.548387050628662</v>
+        <v>1</v>
       </c>
     </row>
     <row r="76" spans="1:4">
       <c r="A76">
-        <v>-1</v>
+        <v>-3.167999982833862</v>
       </c>
       <c r="B76">
-        <v>0.300000011920929</v>
+        <v>1.228000044822693</v>
       </c>
       <c r="C76">
-        <v>0.699999988079071</v>
+        <v>1.939999938011169</v>
       </c>
       <c r="D76">
-        <v>3.333333253860474</v>
+        <v>2.579804420471191</v>
       </c>
     </row>
     <row r="77" spans="1:4">
       <c r="A77">
-        <v>-1.210000038146973</v>
+        <v>-1.343000054359436</v>
       </c>
       <c r="B77">
-        <v>0.2599999904632568</v>
+        <v>1.343000054359436</v>
       </c>
       <c r="C77">
-        <v>0.9500000476837158</v>
+        <v>0</v>
       </c>
       <c r="D77">
-        <v>4.653846263885498</v>
+        <v>1</v>
       </c>
     </row>
     <row r="78" spans="1:4">
       <c r="A78">
-        <v>-0.4900000095367432</v>
+        <v>-3.069999933242798</v>
       </c>
       <c r="B78">
-        <v>0.2700000107288361</v>
+        <v>1</v>
       </c>
       <c r="C78">
-        <v>0.2199999988079071</v>
+        <v>2.069999933242798</v>
       </c>
       <c r="D78">
-        <v>1.814814805984497</v>
+        <v>3.069999933242798</v>
       </c>
     </row>
     <row r="79" spans="1:4">
       <c r="A79">
-        <v>-1.129999995231628</v>
+        <v>-4.140999794006348</v>
       </c>
       <c r="B79">
-        <v>0.2599999904632568</v>
+        <v>1</v>
       </c>
       <c r="C79">
-        <v>0.8700000047683716</v>
+        <v>3.140999794006348</v>
       </c>
       <c r="D79">
-        <v>4.34615421295166</v>
+        <v>4.140999794006348</v>
       </c>
     </row>
     <row r="80" spans="1:4">
       <c r="A80">
-        <v>-1.039999961853027</v>
+        <v>-1</v>
       </c>
       <c r="B80">
-        <v>0.2599999904632568</v>
+        <v>1</v>
       </c>
       <c r="C80">
-        <v>0.7799999713897705</v>
+        <v>0</v>
       </c>
       <c r="D80">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="81" spans="1:4">
       <c r="A81">
-        <v>-0.4900000095367432</v>
+        <v>-1</v>
       </c>
       <c r="B81">
-        <v>0.4900000095367432</v>
+        <v>1</v>
       </c>
       <c r="C81">
         <v>0</v>
@@ -1525,156 +1525,156 @@
     </row>
     <row r="82" spans="1:4">
       <c r="A82">
-        <v>-0.6800000071525574</v>
+        <v>-2.733999967575073</v>
       </c>
       <c r="B82">
-        <v>0.3799999952316284</v>
+        <v>1.516999959945679</v>
       </c>
       <c r="C82">
-        <v>0.300000011920929</v>
+        <v>1.217000007629395</v>
       </c>
       <c r="D82">
-        <v>1.78947377204895</v>
+        <v>1.802241325378418</v>
       </c>
     </row>
     <row r="83" spans="1:4">
       <c r="A83">
-        <v>-2.410000085830688</v>
+        <v>-9.625</v>
       </c>
       <c r="B83">
-        <v>0.4000000059604645</v>
+        <v>1.60099995136261</v>
       </c>
       <c r="C83">
-        <v>2.009999990463257</v>
+        <v>8.02400016784668</v>
       </c>
       <c r="D83">
-        <v>6.025000095367432</v>
+        <v>6.011868000030518</v>
       </c>
     </row>
     <row r="84" spans="1:4">
       <c r="A84">
-        <v>-1</v>
+        <v>-6.254000186920166</v>
       </c>
       <c r="B84">
-        <v>0.4300000071525574</v>
+        <v>1.396000027656555</v>
       </c>
       <c r="C84">
-        <v>0.5699999928474426</v>
+        <v>4.8580002784729</v>
       </c>
       <c r="D84">
-        <v>2.325581312179565</v>
+        <v>4.479942798614502</v>
       </c>
     </row>
     <row r="85" spans="1:4">
       <c r="A85">
-        <v>-0.3899999856948853</v>
+        <v>-4.688000202178955</v>
       </c>
       <c r="B85">
-        <v>0.3100000023841858</v>
+        <v>2.687999963760376</v>
       </c>
       <c r="C85">
-        <v>0.07999998331069946</v>
+        <v>2.000000238418579</v>
       </c>
       <c r="D85">
-        <v>1.25806450843811</v>
+        <v>1.74404776096344</v>
       </c>
     </row>
     <row r="86" spans="1:4">
       <c r="A86">
-        <v>-0.3400000035762787</v>
+        <v>-1</v>
       </c>
       <c r="B86">
-        <v>0.25</v>
+        <v>1</v>
       </c>
       <c r="C86">
-        <v>0.09000000357627869</v>
+        <v>0</v>
       </c>
       <c r="D86">
-        <v>1.360000014305115</v>
+        <v>1</v>
       </c>
     </row>
     <row r="87" spans="1:4">
       <c r="A87">
-        <v>-0.8199999928474426</v>
+        <v>-1.730000019073486</v>
       </c>
       <c r="B87">
-        <v>0.3600000143051147</v>
+        <v>1.730000019073486</v>
       </c>
       <c r="C87">
-        <v>0.4599999785423279</v>
+        <v>0</v>
       </c>
       <c r="D87">
-        <v>2.277777671813965</v>
+        <v>1</v>
       </c>
     </row>
     <row r="88" spans="1:4">
       <c r="A88">
-        <v>-2.410000085830688</v>
+        <v>-3.539000034332275</v>
       </c>
       <c r="B88">
-        <v>0.300000011920929</v>
+        <v>1</v>
       </c>
       <c r="C88">
-        <v>2.110000133514404</v>
+        <v>2.539000034332275</v>
       </c>
       <c r="D88">
-        <v>8.033332824707031</v>
+        <v>3.539000034332275</v>
       </c>
     </row>
     <row r="89" spans="1:4">
       <c r="A89">
-        <v>-0.5</v>
+        <v>-1</v>
       </c>
       <c r="B89">
-        <v>0.3100000023841858</v>
+        <v>1</v>
       </c>
       <c r="C89">
-        <v>0.1899999976158142</v>
+        <v>0</v>
       </c>
       <c r="D89">
-        <v>1.612903237342834</v>
+        <v>1</v>
       </c>
     </row>
     <row r="90" spans="1:4">
       <c r="A90">
-        <v>-0.3899999856948853</v>
+        <v>-1.74399995803833</v>
       </c>
       <c r="B90">
-        <v>0.25</v>
+        <v>1.526999950408936</v>
       </c>
       <c r="C90">
-        <v>0.1399999856948853</v>
+        <v>0.2170000076293945</v>
       </c>
       <c r="D90">
-        <v>1.559999942779541</v>
+        <v>1.142108678817749</v>
       </c>
     </row>
     <row r="91" spans="1:4">
       <c r="A91">
-        <v>-0.5799999833106995</v>
+        <v>-1.842000007629395</v>
       </c>
       <c r="B91">
-        <v>0.4300000071525574</v>
+        <v>1.223999977111816</v>
       </c>
       <c r="C91">
-        <v>0.1499999761581421</v>
+        <v>0.6180000305175781</v>
       </c>
       <c r="D91">
-        <v>1.34883713722229</v>
+        <v>1.504902005195618</v>
       </c>
     </row>
     <row r="92" spans="1:4">
       <c r="A92">
-        <v>-0.4000000059604645</v>
+        <v>-2.342000007629395</v>
       </c>
       <c r="B92">
-        <v>0.3799999952316284</v>
+        <v>2.342000007629395</v>
       </c>
       <c r="C92">
-        <v>0.02000001072883606</v>
+        <v>0</v>
       </c>
       <c r="D92">
-        <v>1.052631616592407</v>
+        <v>1</v>
       </c>
     </row>
     <row r="93" spans="1:4">
@@ -1693,30 +1693,58 @@
     </row>
     <row r="94" spans="1:4">
       <c r="A94">
-        <v>-0.4099999964237213</v>
+        <v>-1.121000051498413</v>
       </c>
       <c r="B94">
-        <v>0.2700000107288361</v>
+        <v>1.121000051498413</v>
       </c>
       <c r="C94">
-        <v>0.1399999856948853</v>
+        <v>0</v>
       </c>
       <c r="D94">
-        <v>1.518518447875977</v>
+        <v>1</v>
       </c>
     </row>
     <row r="95" spans="1:4">
       <c r="A95">
-        <v>-3.930000066757202</v>
+        <v>-1.315999984741211</v>
       </c>
       <c r="B95">
-        <v>1</v>
+        <v>1.315999984741211</v>
       </c>
       <c r="C95">
-        <v>2.930000066757202</v>
+        <v>0</v>
       </c>
       <c r="D95">
-        <v>3.930000066757202</v>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4">
+      <c r="A96">
+        <v>-1.264999985694885</v>
+      </c>
+      <c r="B96">
+        <v>1</v>
+      </c>
+      <c r="C96">
+        <v>0.2649999856948853</v>
+      </c>
+      <c r="D96">
+        <v>1.264999985694885</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4">
+      <c r="A97">
+        <v>-11.73400020599365</v>
+      </c>
+      <c r="B97">
+        <v>1.049999952316284</v>
+      </c>
+      <c r="C97">
+        <v>10.68400001525879</v>
+      </c>
+      <c r="D97">
+        <v>11.17523860931396</v>
       </c>
     </row>
   </sheetData>

</xml_diff>